<commit_message>
Multiple sentence functionality up and running. Also clarified that ADJ NOUN surprisal is at the NOUN. README updated with this information.
</commit_message>
<xml_diff>
--- a/stimuli/multi_sent.xlsx
+++ b/stimuli/multi_sent.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
   <si>
     <t xml:space="preserve">sent1</t>
   </si>
@@ -28,6 +28,24 @@
     <t xml:space="preserve">sent2</t>
   </si>
   <si>
+    <t xml:space="preserve">The man will criticize the brochure. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">And then, he will read the brochure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The man will fold the brochure. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The man will kick the gate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">And then, he will lean on the gate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The man will shut the gate.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The boy will inspect the broken zipper. </t>
   </si>
   <si>
@@ -35,24 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">The boy will fix the broken zipper.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The man will criticize the brochure. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">And then, he will read the brochure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The man will fold the brochure. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The man will kick the gate. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">And then, he will lean on the gate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The man will shut the gate.</t>
   </si>
   <si>
     <t xml:space="preserve">The child will tap the ketchup bottle. </t>
@@ -411,18 +411,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.5612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="12.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="12.3724489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,465 +483,449 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65" s="1" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>